<commit_message>
Correcao modelos pentaho. Todos os campos finalizados
</commit_message>
<xml_diff>
--- a/Modelos_V2/tabela1_padrao_matricula.xlsx
+++ b/Modelos_V2/tabela1_padrao_matricula.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19126"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mansouza\Documents\www\TrajetoriaEscolar\Modelos_V2\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{CF7200C0-B6E2-4745-9B62-5435C8296E80}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12945"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12945" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Matrículas-Total" sheetId="1" r:id="rId1"/>
@@ -186,14 +192,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-  </numFmts>
-  <fonts count="25">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -229,159 +229,8 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="43">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -408,25 +257,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="3" tint="0.599993896298105"/>
+        <fgColor theme="3" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="3" tint="0.599993896298105"/>
+        <fgColor theme="3" tint="0.59999389629810485"/>
         <bgColor rgb="FFB3A2C7"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.59999389629810485"/>
         <bgColor rgb="FFB3A2C7"/>
       </patternFill>
     </fill>
@@ -438,204 +287,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor rgb="FF95B3D7"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="20">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -774,260 +437,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="42" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="16" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="19" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="21" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="20" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1038,9 +453,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1049,11 +461,74 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1061,110 +536,18 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="60% - Accent6" xfId="1" builtinId="52"/>
-    <cellStyle name="40% - Accent6" xfId="2" builtinId="51"/>
-    <cellStyle name="60% - Accent5" xfId="3" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="4" builtinId="49"/>
-    <cellStyle name="40% - Accent5" xfId="5" builtinId="47"/>
-    <cellStyle name="20% - Accent5" xfId="6" builtinId="46"/>
-    <cellStyle name="60% - Accent4" xfId="7" builtinId="44"/>
-    <cellStyle name="Accent5" xfId="8" builtinId="45"/>
-    <cellStyle name="40% - Accent4" xfId="9" builtinId="43"/>
-    <cellStyle name="Accent4" xfId="10" builtinId="41"/>
-    <cellStyle name="Linked Cell" xfId="11" builtinId="24"/>
-    <cellStyle name="40% - Accent3" xfId="12" builtinId="39"/>
-    <cellStyle name="60% - Accent2" xfId="13" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="14" builtinId="37"/>
-    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="20% - Accent2" xfId="16" builtinId="34"/>
-    <cellStyle name="Accent2" xfId="17" builtinId="33"/>
-    <cellStyle name="40% - Accent1" xfId="18" builtinId="31"/>
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30"/>
-    <cellStyle name="Accent1" xfId="20" builtinId="29"/>
-    <cellStyle name="Neutral" xfId="21" builtinId="28"/>
-    <cellStyle name="60% - Accent1" xfId="22" builtinId="32"/>
-    <cellStyle name="Bad" xfId="23" builtinId="27"/>
-    <cellStyle name="20% - Accent4" xfId="24" builtinId="42"/>
-    <cellStyle name="Total" xfId="25" builtinId="25"/>
-    <cellStyle name="Output" xfId="26" builtinId="21"/>
-    <cellStyle name="Currency" xfId="27" builtinId="4"/>
-    <cellStyle name="20% - Accent3" xfId="28" builtinId="38"/>
-    <cellStyle name="Note" xfId="29" builtinId="10"/>
-    <cellStyle name="Input" xfId="30" builtinId="20"/>
-    <cellStyle name="Heading 4" xfId="31" builtinId="19"/>
-    <cellStyle name="Calculation" xfId="32" builtinId="22"/>
-    <cellStyle name="Good" xfId="33" builtinId="26"/>
-    <cellStyle name="Heading 3" xfId="34" builtinId="18"/>
-    <cellStyle name="CExplanatory Text" xfId="35" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="36" builtinId="16"/>
-    <cellStyle name="Comma [0]" xfId="37" builtinId="6"/>
-    <cellStyle name="20% - Accent6" xfId="38" builtinId="50"/>
-    <cellStyle name="Title" xfId="39" builtinId="15"/>
-    <cellStyle name="Currency [0]" xfId="40" builtinId="7"/>
-    <cellStyle name="Warning Text" xfId="41" builtinId="11"/>
-    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9"/>
-    <cellStyle name="Heading 2" xfId="43" builtinId="17"/>
-    <cellStyle name="Comma" xfId="44" builtinId="3"/>
-    <cellStyle name="Check Cell" xfId="45" builtinId="23"/>
-    <cellStyle name="60% - Accent3" xfId="46" builtinId="40"/>
-    <cellStyle name="Percent" xfId="47" builtinId="5"/>
-    <cellStyle name="Hyperlink" xfId="48" builtinId="8"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1422,269 +805,269 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:I4"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83333333333333" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.3333333333333" customWidth="1"/>
-    <col min="2" max="2" width="7.5" customWidth="1"/>
-    <col min="3" max="3" width="9.5" customWidth="1"/>
-    <col min="4" max="4" width="10.3333333333333" customWidth="1"/>
-    <col min="5" max="5" width="11.5" customWidth="1"/>
-    <col min="6" max="6" width="39.6666666666667" customWidth="1"/>
-    <col min="7" max="7" width="11.6666666666667" customWidth="1"/>
-    <col min="8" max="8" width="14.5" customWidth="1"/>
-    <col min="9" max="9" width="21.1666666666667" customWidth="1"/>
-    <col min="10" max="22" width="20.6666666666667" customWidth="1"/>
+    <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.42578125" customWidth="1"/>
+    <col min="3" max="3" width="9.42578125" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" customWidth="1"/>
+    <col min="6" max="6" width="39.7109375" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" customWidth="1"/>
+    <col min="8" max="8" width="14.42578125" customWidth="1"/>
+    <col min="9" max="9" width="21.140625" customWidth="1"/>
+    <col min="10" max="22" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="30"/>
-      <c r="J1" s="31" t="s">
-        <v>1</v>
-      </c>
-      <c r="K1" s="31"/>
-      <c r="L1" s="31"/>
-      <c r="M1" s="31"/>
-      <c r="N1" s="31"/>
-      <c r="O1" s="31"/>
-      <c r="P1" s="31"/>
-      <c r="Q1" s="31"/>
-      <c r="R1" s="31"/>
-      <c r="S1" s="31"/>
-      <c r="T1" s="31"/>
-      <c r="U1" s="31"/>
-      <c r="V1" s="31"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="27"/>
+      <c r="J1" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="K1" s="28"/>
+      <c r="L1" s="28"/>
+      <c r="M1" s="28"/>
+      <c r="N1" s="28"/>
+      <c r="O1" s="28"/>
+      <c r="P1" s="28"/>
+      <c r="Q1" s="28"/>
+      <c r="R1" s="28"/>
+      <c r="S1" s="28"/>
+      <c r="T1" s="28"/>
+      <c r="U1" s="28"/>
+      <c r="V1" s="28"/>
     </row>
-    <row r="2" spans="10:22">
-      <c r="J2" s="22" t="s">
+    <row r="2" spans="1:22">
+      <c r="J2" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="K2" s="22"/>
-      <c r="L2" s="22"/>
-      <c r="M2" s="22"/>
-      <c r="N2" s="22"/>
-      <c r="O2" s="22"/>
-      <c r="P2" s="22"/>
-      <c r="Q2" s="22"/>
-      <c r="R2" s="22"/>
-      <c r="S2" s="38" t="s">
+      <c r="K2" s="29"/>
+      <c r="L2" s="29"/>
+      <c r="M2" s="29"/>
+      <c r="N2" s="29"/>
+      <c r="O2" s="29"/>
+      <c r="P2" s="29"/>
+      <c r="Q2" s="29"/>
+      <c r="R2" s="29"/>
+      <c r="S2" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="T2" s="38"/>
-      <c r="U2" s="38"/>
-      <c r="V2" s="38"/>
+      <c r="T2" s="30"/>
+      <c r="U2" s="30"/>
+      <c r="V2" s="30"/>
     </row>
-    <row r="3" spans="1:22">
-      <c r="A3" s="28"/>
-      <c r="B3" s="29"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
-      <c r="F3" s="29"/>
-      <c r="G3" s="29"/>
-      <c r="H3" s="29"/>
-      <c r="I3" s="32"/>
-      <c r="J3" s="33" t="s">
+    <row r="3" spans="1:22" ht="15.75">
+      <c r="A3" s="19"/>
+      <c r="B3" s="20"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="20"/>
+      <c r="H3" s="20"/>
+      <c r="I3" s="21"/>
+      <c r="J3" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="K3" s="34"/>
-      <c r="L3" s="34"/>
-      <c r="M3" s="34"/>
-      <c r="N3" s="36"/>
-      <c r="O3" s="22" t="s">
+      <c r="K3" s="32"/>
+      <c r="L3" s="32"/>
+      <c r="M3" s="32"/>
+      <c r="N3" s="33"/>
+      <c r="O3" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="P3" s="22"/>
-      <c r="Q3" s="22"/>
-      <c r="R3" s="22"/>
-      <c r="S3" s="39"/>
-      <c r="T3" s="39"/>
-      <c r="U3" s="39"/>
-      <c r="V3" s="39"/>
+      <c r="P3" s="29"/>
+      <c r="Q3" s="29"/>
+      <c r="R3" s="29"/>
+      <c r="S3" s="25"/>
+      <c r="T3" s="25"/>
+      <c r="U3" s="25"/>
+      <c r="V3" s="25"/>
     </row>
-    <row r="4" spans="1:22">
-      <c r="A4" s="28" t="s">
+    <row r="4" spans="1:22" ht="15.75">
+      <c r="A4" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="29" t="s">
+      <c r="B4" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="29" t="s">
+      <c r="C4" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="29" t="s">
+      <c r="D4" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="29" t="s">
+      <c r="E4" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="F4" s="29" t="s">
+      <c r="F4" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="G4" s="29" t="s">
+      <c r="G4" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="H4" s="29" t="s">
+      <c r="H4" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="I4" s="32" t="s">
+      <c r="I4" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="J4" s="13" t="s">
+      <c r="J4" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="K4" s="13" t="s">
+      <c r="K4" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="L4" s="13" t="s">
+      <c r="L4" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="M4" s="13" t="s">
+      <c r="M4" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="N4" s="13" t="s">
+      <c r="N4" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="O4" s="13" t="s">
+      <c r="O4" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="P4" s="13" t="s">
+      <c r="P4" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="Q4" s="13" t="s">
+      <c r="Q4" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="R4" s="13" t="s">
+      <c r="R4" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="S4" s="38" t="s">
+      <c r="S4" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="T4" s="38" t="s">
+      <c r="T4" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="U4" s="38" t="s">
+      <c r="U4" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="V4" s="38" t="s">
+      <c r="V4" s="24" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:22">
-      <c r="A5" s="18">
+      <c r="A5" s="12">
         <v>11000465</v>
       </c>
-      <c r="B5" s="19" t="s">
+      <c r="B5" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="C5" s="19" t="s">
+      <c r="C5" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="D5" s="19" t="s">
+      <c r="D5" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="E5" s="19" t="s">
+      <c r="E5" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="F5" s="19" t="s">
+      <c r="F5" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="G5" s="19" t="s">
+      <c r="G5" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="H5" s="19" t="s">
+      <c r="H5" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="I5" s="24" t="s">
+      <c r="I5" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="J5" s="35">
-        <v>1</v>
-      </c>
-      <c r="K5" s="35">
+      <c r="J5" s="22">
+        <v>1</v>
+      </c>
+      <c r="K5" s="22">
         <v>2</v>
       </c>
-      <c r="L5" s="35">
+      <c r="L5" s="22">
         <v>3</v>
       </c>
-      <c r="M5" s="35">
+      <c r="M5" s="22">
         <v>4</v>
       </c>
-      <c r="N5" s="35">
+      <c r="N5" s="22">
         <v>5</v>
       </c>
-      <c r="O5" s="35">
+      <c r="O5" s="22">
         <v>6</v>
       </c>
-      <c r="P5" s="35">
+      <c r="P5" s="22">
         <v>7</v>
       </c>
-      <c r="Q5" s="35">
+      <c r="Q5" s="22">
         <v>8</v>
       </c>
-      <c r="R5" s="35">
+      <c r="R5" s="22">
         <v>9</v>
       </c>
-      <c r="S5" s="35">
+      <c r="S5" s="22">
         <v>10</v>
       </c>
-      <c r="T5" s="35">
+      <c r="T5" s="22">
         <v>11</v>
       </c>
-      <c r="U5" s="35">
+      <c r="U5" s="22">
         <v>12</v>
       </c>
-      <c r="V5" s="35">
+      <c r="V5" s="22">
         <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:22">
-      <c r="A6" s="20">
+      <c r="A6" s="14">
         <v>11000201</v>
       </c>
-      <c r="B6" s="21" t="s">
+      <c r="B6" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="C6" s="21" t="s">
+      <c r="C6" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="D6" s="21" t="s">
+      <c r="D6" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="E6" s="21" t="s">
+      <c r="E6" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="F6" s="21" t="s">
+      <c r="F6" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="G6" s="21" t="s">
+      <c r="G6" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="H6" s="21" t="s">
+      <c r="H6" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="I6" s="25" t="s">
+      <c r="I6" s="18" t="s">
         <v>38</v>
       </c>
       <c r="J6">
@@ -1728,31 +1111,31 @@
       </c>
     </row>
     <row r="7" spans="1:22">
-      <c r="A7" s="20">
+      <c r="A7" s="14">
         <v>11000260</v>
       </c>
-      <c r="B7" s="21" t="s">
+      <c r="B7" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="21" t="s">
+      <c r="C7" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="D7" s="21" t="s">
+      <c r="D7" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="E7" s="21" t="s">
+      <c r="E7" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="F7" s="21" t="s">
+      <c r="F7" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="G7" s="21" t="s">
+      <c r="G7" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="H7" s="21" t="s">
+      <c r="H7" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="I7" s="25" t="s">
+      <c r="I7" s="18" t="s">
         <v>38</v>
       </c>
       <c r="J7">
@@ -1796,31 +1179,31 @@
       </c>
     </row>
     <row r="8" spans="1:22">
-      <c r="A8" s="20">
+      <c r="A8" s="14">
         <v>11000317</v>
       </c>
-      <c r="B8" s="21" t="s">
+      <c r="B8" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="21" t="s">
+      <c r="C8" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="D8" s="21" t="s">
+      <c r="D8" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="E8" s="21" t="s">
+      <c r="E8" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="F8" s="21" t="s">
+      <c r="F8" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="G8" s="21" t="s">
+      <c r="G8" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="H8" s="21" t="s">
+      <c r="H8" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="I8" s="25" t="s">
+      <c r="I8" s="18" t="s">
         <v>38</v>
       </c>
       <c r="J8">
@@ -1863,8 +1246,8 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="13:13">
-      <c r="M10" s="37"/>
+    <row r="10" spans="1:22">
+      <c r="M10" s="23"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -1876,703 +1259,701 @@
     <mergeCell ref="O3:R3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="portrait"/>
-  <headerFooter/>
+  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:CI8"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" topLeftCell="G1" workbookViewId="0">
+    <sheetView topLeftCell="G1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83333333333333" defaultRowHeight="15.75" outlineLevelRow="7"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.3333333333333" customWidth="1"/>
-    <col min="2" max="2" width="7.5" customWidth="1"/>
-    <col min="3" max="3" width="9.5" customWidth="1"/>
-    <col min="4" max="4" width="10.3333333333333" customWidth="1"/>
-    <col min="5" max="5" width="11.5" customWidth="1"/>
-    <col min="6" max="6" width="39.6666666666667" customWidth="1"/>
-    <col min="7" max="7" width="11.6666666666667" customWidth="1"/>
-    <col min="8" max="8" width="14.5" customWidth="1"/>
-    <col min="9" max="9" width="21.1666666666667" customWidth="1"/>
-    <col min="10" max="10" width="15.3333333333333" customWidth="1"/>
-    <col min="11" max="11" width="7.5" customWidth="1"/>
-    <col min="12" max="12" width="5.83333333333333" customWidth="1"/>
-    <col min="13" max="13" width="6.33333333333333" customWidth="1"/>
-    <col min="14" max="14" width="8.66666666666667" customWidth="1"/>
+    <col min="1" max="1" width="10.28515625" customWidth="1"/>
+    <col min="2" max="2" width="7.42578125" customWidth="1"/>
+    <col min="3" max="3" width="9.42578125" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" customWidth="1"/>
+    <col min="6" max="6" width="39.7109375" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" customWidth="1"/>
+    <col min="8" max="8" width="14.42578125" customWidth="1"/>
+    <col min="9" max="9" width="21.140625" customWidth="1"/>
+    <col min="10" max="10" width="15.28515625" customWidth="1"/>
+    <col min="11" max="11" width="7.42578125" customWidth="1"/>
+    <col min="12" max="12" width="5.85546875" customWidth="1"/>
+    <col min="13" max="13" width="6.28515625" customWidth="1"/>
+    <col min="14" max="14" width="8.7109375" customWidth="1"/>
     <col min="15" max="15" width="9" customWidth="1"/>
-    <col min="16" max="16" width="14.5" customWidth="1"/>
-    <col min="17" max="17" width="7.5" customWidth="1"/>
-    <col min="18" max="18" width="5.83333333333333" customWidth="1"/>
-    <col min="19" max="19" width="6.33333333333333" customWidth="1"/>
-    <col min="20" max="20" width="8.66666666666667" customWidth="1"/>
+    <col min="16" max="16" width="14.42578125" customWidth="1"/>
+    <col min="17" max="17" width="7.42578125" customWidth="1"/>
+    <col min="18" max="18" width="5.85546875" customWidth="1"/>
+    <col min="19" max="19" width="6.28515625" customWidth="1"/>
+    <col min="20" max="20" width="8.7109375" customWidth="1"/>
     <col min="21" max="21" width="9" customWidth="1"/>
-    <col min="22" max="22" width="14.5" customWidth="1"/>
-    <col min="23" max="23" width="7.5" customWidth="1"/>
-    <col min="24" max="24" width="5.83333333333333" customWidth="1"/>
-    <col min="25" max="25" width="6.33333333333333" customWidth="1"/>
-    <col min="26" max="26" width="8.66666666666667" customWidth="1"/>
+    <col min="22" max="22" width="14.42578125" customWidth="1"/>
+    <col min="23" max="23" width="7.42578125" customWidth="1"/>
+    <col min="24" max="24" width="5.85546875" customWidth="1"/>
+    <col min="25" max="25" width="6.28515625" customWidth="1"/>
+    <col min="26" max="26" width="8.7109375" customWidth="1"/>
     <col min="27" max="27" width="9" customWidth="1"/>
-    <col min="28" max="28" width="14.5" customWidth="1"/>
-    <col min="29" max="29" width="7.5" customWidth="1"/>
-    <col min="30" max="30" width="5.83333333333333" customWidth="1"/>
-    <col min="31" max="31" width="6.33333333333333" customWidth="1"/>
-    <col min="32" max="32" width="8.66666666666667" customWidth="1"/>
+    <col min="28" max="28" width="14.42578125" customWidth="1"/>
+    <col min="29" max="29" width="7.42578125" customWidth="1"/>
+    <col min="30" max="30" width="5.85546875" customWidth="1"/>
+    <col min="31" max="31" width="6.28515625" customWidth="1"/>
+    <col min="32" max="32" width="8.7109375" customWidth="1"/>
     <col min="33" max="33" width="9" customWidth="1"/>
-    <col min="34" max="34" width="14.5" customWidth="1"/>
-    <col min="35" max="35" width="7.5" customWidth="1"/>
-    <col min="36" max="36" width="5.83333333333333" customWidth="1"/>
-    <col min="37" max="37" width="6.33333333333333" customWidth="1"/>
-    <col min="38" max="38" width="8.66666666666667" customWidth="1"/>
+    <col min="34" max="34" width="14.42578125" customWidth="1"/>
+    <col min="35" max="35" width="7.42578125" customWidth="1"/>
+    <col min="36" max="36" width="5.85546875" customWidth="1"/>
+    <col min="37" max="37" width="6.28515625" customWidth="1"/>
+    <col min="38" max="38" width="8.7109375" customWidth="1"/>
     <col min="39" max="39" width="9" customWidth="1"/>
-    <col min="40" max="40" width="14.5" customWidth="1"/>
-    <col min="41" max="41" width="7.5" customWidth="1"/>
-    <col min="42" max="42" width="5.83333333333333" customWidth="1"/>
-    <col min="43" max="43" width="6.33333333333333" customWidth="1"/>
-    <col min="44" max="44" width="8.66666666666667" customWidth="1"/>
+    <col min="40" max="40" width="14.42578125" customWidth="1"/>
+    <col min="41" max="41" width="7.42578125" customWidth="1"/>
+    <col min="42" max="42" width="5.85546875" customWidth="1"/>
+    <col min="43" max="43" width="6.28515625" customWidth="1"/>
+    <col min="44" max="44" width="8.7109375" customWidth="1"/>
     <col min="45" max="45" width="9" customWidth="1"/>
-    <col min="46" max="46" width="14.5" customWidth="1"/>
-    <col min="47" max="47" width="7.5" customWidth="1"/>
-    <col min="48" max="48" width="5.83333333333333" customWidth="1"/>
-    <col min="49" max="49" width="6.33333333333333" customWidth="1"/>
-    <col min="50" max="50" width="8.66666666666667" customWidth="1"/>
+    <col min="46" max="46" width="14.42578125" customWidth="1"/>
+    <col min="47" max="47" width="7.42578125" customWidth="1"/>
+    <col min="48" max="48" width="5.85546875" customWidth="1"/>
+    <col min="49" max="49" width="6.28515625" customWidth="1"/>
+    <col min="50" max="50" width="8.7109375" customWidth="1"/>
     <col min="51" max="51" width="9" customWidth="1"/>
-    <col min="52" max="52" width="14.5" customWidth="1"/>
-    <col min="53" max="53" width="7.5" customWidth="1"/>
-    <col min="54" max="54" width="5.83333333333333" customWidth="1"/>
-    <col min="55" max="55" width="6.33333333333333" customWidth="1"/>
-    <col min="56" max="56" width="8.66666666666667" customWidth="1"/>
+    <col min="52" max="52" width="14.42578125" customWidth="1"/>
+    <col min="53" max="53" width="7.42578125" customWidth="1"/>
+    <col min="54" max="54" width="5.85546875" customWidth="1"/>
+    <col min="55" max="55" width="6.28515625" customWidth="1"/>
+    <col min="56" max="56" width="8.7109375" customWidth="1"/>
     <col min="57" max="57" width="9" customWidth="1"/>
-    <col min="58" max="58" width="14.5" customWidth="1"/>
-    <col min="59" max="59" width="7.5" customWidth="1"/>
-    <col min="60" max="60" width="5.83333333333333" customWidth="1"/>
-    <col min="61" max="61" width="6.33333333333333" customWidth="1"/>
-    <col min="62" max="62" width="8.66666666666667" customWidth="1"/>
+    <col min="58" max="58" width="14.42578125" customWidth="1"/>
+    <col min="59" max="59" width="7.42578125" customWidth="1"/>
+    <col min="60" max="60" width="5.85546875" customWidth="1"/>
+    <col min="61" max="61" width="6.28515625" customWidth="1"/>
+    <col min="62" max="62" width="8.7109375" customWidth="1"/>
     <col min="63" max="63" width="9" customWidth="1"/>
-    <col min="64" max="64" width="14.5" customWidth="1"/>
-    <col min="65" max="65" width="7.5" customWidth="1"/>
-    <col min="66" max="66" width="5.83333333333333" customWidth="1"/>
-    <col min="67" max="67" width="6.33333333333333" customWidth="1"/>
-    <col min="68" max="68" width="8.66666666666667" customWidth="1"/>
+    <col min="64" max="64" width="14.42578125" customWidth="1"/>
+    <col min="65" max="65" width="7.42578125" customWidth="1"/>
+    <col min="66" max="66" width="5.85546875" customWidth="1"/>
+    <col min="67" max="67" width="6.28515625" customWidth="1"/>
+    <col min="68" max="68" width="8.7109375" customWidth="1"/>
     <col min="69" max="69" width="9" customWidth="1"/>
-    <col min="70" max="70" width="14.5" customWidth="1"/>
-    <col min="71" max="71" width="7.5" customWidth="1"/>
-    <col min="72" max="72" width="5.83333333333333" customWidth="1"/>
-    <col min="73" max="73" width="6.33333333333333" customWidth="1"/>
-    <col min="74" max="74" width="8.66666666666667" customWidth="1"/>
+    <col min="70" max="70" width="14.42578125" customWidth="1"/>
+    <col min="71" max="71" width="7.42578125" customWidth="1"/>
+    <col min="72" max="72" width="5.85546875" customWidth="1"/>
+    <col min="73" max="73" width="6.28515625" customWidth="1"/>
+    <col min="74" max="74" width="8.7109375" customWidth="1"/>
     <col min="75" max="75" width="9" customWidth="1"/>
-    <col min="76" max="76" width="14.5" customWidth="1"/>
-    <col min="77" max="77" width="7.5" customWidth="1"/>
-    <col min="78" max="78" width="5.83333333333333" customWidth="1"/>
-    <col min="79" max="79" width="6.33333333333333" customWidth="1"/>
-    <col min="80" max="80" width="8.66666666666667" customWidth="1"/>
+    <col min="76" max="76" width="14.42578125" customWidth="1"/>
+    <col min="77" max="77" width="7.42578125" customWidth="1"/>
+    <col min="78" max="78" width="5.85546875" customWidth="1"/>
+    <col min="79" max="79" width="6.28515625" customWidth="1"/>
+    <col min="80" max="80" width="8.7109375" customWidth="1"/>
     <col min="81" max="81" width="9" customWidth="1"/>
-    <col min="82" max="82" width="14.5" customWidth="1"/>
-    <col min="83" max="83" width="7.5" customWidth="1"/>
-    <col min="84" max="84" width="5.83333333333333" customWidth="1"/>
-    <col min="85" max="85" width="6.33333333333333" customWidth="1"/>
-    <col min="86" max="86" width="8.66666666666667" customWidth="1"/>
+    <col min="82" max="82" width="14.42578125" customWidth="1"/>
+    <col min="83" max="83" width="7.42578125" customWidth="1"/>
+    <col min="84" max="84" width="5.85546875" customWidth="1"/>
+    <col min="85" max="85" width="6.28515625" customWidth="1"/>
+    <col min="86" max="86" width="8.7109375" customWidth="1"/>
     <col min="87" max="87" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15" customHeight="1" spans="1:87">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:87" ht="15" customHeight="1">
+      <c r="A1" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="22" t="s">
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
+      <c r="I1" s="34"/>
+      <c r="J1" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="K1" s="22"/>
-      <c r="L1" s="22"/>
-      <c r="M1" s="22"/>
-      <c r="N1" s="22"/>
-      <c r="O1" s="22"/>
-      <c r="P1" s="22"/>
-      <c r="Q1" s="22"/>
-      <c r="R1" s="22"/>
-      <c r="S1" s="22"/>
-      <c r="T1" s="22"/>
-      <c r="U1" s="22"/>
-      <c r="V1" s="22"/>
-      <c r="W1" s="22"/>
-      <c r="X1" s="22"/>
-      <c r="Y1" s="22"/>
-      <c r="Z1" s="22"/>
-      <c r="AA1" s="22"/>
-      <c r="AB1" s="22"/>
-      <c r="AC1" s="22"/>
-      <c r="AD1" s="22"/>
-      <c r="AE1" s="22"/>
-      <c r="AF1" s="22"/>
-      <c r="AG1" s="22"/>
-      <c r="AH1" s="22"/>
-      <c r="AI1" s="22"/>
-      <c r="AJ1" s="22"/>
-      <c r="AK1" s="22"/>
-      <c r="AL1" s="22"/>
-      <c r="AM1" s="22"/>
-      <c r="AN1" s="22"/>
-      <c r="AO1" s="22"/>
-      <c r="AP1" s="22"/>
-      <c r="AQ1" s="22"/>
-      <c r="AR1" s="22"/>
-      <c r="AS1" s="22"/>
-      <c r="AT1" s="22"/>
-      <c r="AU1" s="22"/>
-      <c r="AV1" s="22"/>
-      <c r="AW1" s="22"/>
-      <c r="AX1" s="22"/>
-      <c r="AY1" s="22"/>
-      <c r="AZ1" s="22"/>
-      <c r="BA1" s="22"/>
-      <c r="BB1" s="22"/>
-      <c r="BC1" s="22"/>
-      <c r="BD1" s="22"/>
-      <c r="BE1" s="22"/>
-      <c r="BF1" s="22"/>
-      <c r="BG1" s="22"/>
-      <c r="BH1" s="22"/>
-      <c r="BI1" s="22"/>
-      <c r="BJ1" s="22"/>
-      <c r="BK1" s="22"/>
-      <c r="BL1" s="22" t="s">
+      <c r="K1" s="29"/>
+      <c r="L1" s="29"/>
+      <c r="M1" s="29"/>
+      <c r="N1" s="29"/>
+      <c r="O1" s="29"/>
+      <c r="P1" s="29"/>
+      <c r="Q1" s="29"/>
+      <c r="R1" s="29"/>
+      <c r="S1" s="29"/>
+      <c r="T1" s="29"/>
+      <c r="U1" s="29"/>
+      <c r="V1" s="29"/>
+      <c r="W1" s="29"/>
+      <c r="X1" s="29"/>
+      <c r="Y1" s="29"/>
+      <c r="Z1" s="29"/>
+      <c r="AA1" s="29"/>
+      <c r="AB1" s="29"/>
+      <c r="AC1" s="29"/>
+      <c r="AD1" s="29"/>
+      <c r="AE1" s="29"/>
+      <c r="AF1" s="29"/>
+      <c r="AG1" s="29"/>
+      <c r="AH1" s="29"/>
+      <c r="AI1" s="29"/>
+      <c r="AJ1" s="29"/>
+      <c r="AK1" s="29"/>
+      <c r="AL1" s="29"/>
+      <c r="AM1" s="29"/>
+      <c r="AN1" s="29"/>
+      <c r="AO1" s="29"/>
+      <c r="AP1" s="29"/>
+      <c r="AQ1" s="29"/>
+      <c r="AR1" s="29"/>
+      <c r="AS1" s="29"/>
+      <c r="AT1" s="29"/>
+      <c r="AU1" s="29"/>
+      <c r="AV1" s="29"/>
+      <c r="AW1" s="29"/>
+      <c r="AX1" s="29"/>
+      <c r="AY1" s="29"/>
+      <c r="AZ1" s="29"/>
+      <c r="BA1" s="29"/>
+      <c r="BB1" s="29"/>
+      <c r="BC1" s="29"/>
+      <c r="BD1" s="29"/>
+      <c r="BE1" s="29"/>
+      <c r="BF1" s="29"/>
+      <c r="BG1" s="29"/>
+      <c r="BH1" s="29"/>
+      <c r="BI1" s="29"/>
+      <c r="BJ1" s="29"/>
+      <c r="BK1" s="29"/>
+      <c r="BL1" s="29" t="s">
         <v>42</v>
       </c>
-      <c r="BM1" s="22"/>
-      <c r="BN1" s="22"/>
-      <c r="BO1" s="22"/>
-      <c r="BP1" s="22"/>
-      <c r="BQ1" s="22"/>
-      <c r="BR1" s="22"/>
-      <c r="BS1" s="22"/>
-      <c r="BT1" s="22"/>
-      <c r="BU1" s="22"/>
-      <c r="BV1" s="22"/>
-      <c r="BW1" s="22"/>
-      <c r="BX1" s="22"/>
-      <c r="BY1" s="22"/>
-      <c r="BZ1" s="22"/>
-      <c r="CA1" s="22"/>
-      <c r="CB1" s="22"/>
-      <c r="CC1" s="22"/>
-      <c r="CD1" s="22"/>
-      <c r="CE1" s="22"/>
-      <c r="CF1" s="22"/>
-      <c r="CG1" s="22"/>
-      <c r="CH1" s="22"/>
-      <c r="CI1" s="22"/>
+      <c r="BM1" s="29"/>
+      <c r="BN1" s="29"/>
+      <c r="BO1" s="29"/>
+      <c r="BP1" s="29"/>
+      <c r="BQ1" s="29"/>
+      <c r="BR1" s="29"/>
+      <c r="BS1" s="29"/>
+      <c r="BT1" s="29"/>
+      <c r="BU1" s="29"/>
+      <c r="BV1" s="29"/>
+      <c r="BW1" s="29"/>
+      <c r="BX1" s="29"/>
+      <c r="BY1" s="29"/>
+      <c r="BZ1" s="29"/>
+      <c r="CA1" s="29"/>
+      <c r="CB1" s="29"/>
+      <c r="CC1" s="29"/>
+      <c r="CD1" s="29"/>
+      <c r="CE1" s="29"/>
+      <c r="CF1" s="29"/>
+      <c r="CG1" s="29"/>
+      <c r="CH1" s="29"/>
+      <c r="CI1" s="29"/>
     </row>
-    <row r="2" ht="15" customHeight="1" spans="1:87">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="22" t="s">
+    <row r="2" spans="1:87" ht="15" customHeight="1">
+      <c r="A2" s="35"/>
+      <c r="B2" s="35"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="35"/>
+      <c r="I2" s="35"/>
+      <c r="J2" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="22"/>
-      <c r="L2" s="22"/>
-      <c r="M2" s="22"/>
-      <c r="N2" s="22"/>
-      <c r="O2" s="22"/>
-      <c r="P2" s="22"/>
-      <c r="Q2" s="22"/>
-      <c r="R2" s="22"/>
-      <c r="S2" s="22"/>
-      <c r="T2" s="22"/>
-      <c r="U2" s="22"/>
-      <c r="V2" s="22"/>
-      <c r="W2" s="22"/>
-      <c r="X2" s="22"/>
-      <c r="Y2" s="22"/>
-      <c r="Z2" s="22"/>
-      <c r="AA2" s="22"/>
-      <c r="AB2" s="22"/>
-      <c r="AC2" s="22"/>
-      <c r="AD2" s="22"/>
-      <c r="AE2" s="22"/>
-      <c r="AF2" s="22"/>
-      <c r="AG2" s="22"/>
-      <c r="AH2" s="22"/>
-      <c r="AI2" s="22"/>
-      <c r="AJ2" s="22"/>
-      <c r="AK2" s="22"/>
-      <c r="AL2" s="22"/>
-      <c r="AM2" s="22"/>
-      <c r="AN2" s="22" t="s">
+      <c r="K2" s="29"/>
+      <c r="L2" s="29"/>
+      <c r="M2" s="29"/>
+      <c r="N2" s="29"/>
+      <c r="O2" s="29"/>
+      <c r="P2" s="29"/>
+      <c r="Q2" s="29"/>
+      <c r="R2" s="29"/>
+      <c r="S2" s="29"/>
+      <c r="T2" s="29"/>
+      <c r="U2" s="29"/>
+      <c r="V2" s="29"/>
+      <c r="W2" s="29"/>
+      <c r="X2" s="29"/>
+      <c r="Y2" s="29"/>
+      <c r="Z2" s="29"/>
+      <c r="AA2" s="29"/>
+      <c r="AB2" s="29"/>
+      <c r="AC2" s="29"/>
+      <c r="AD2" s="29"/>
+      <c r="AE2" s="29"/>
+      <c r="AF2" s="29"/>
+      <c r="AG2" s="29"/>
+      <c r="AH2" s="29"/>
+      <c r="AI2" s="29"/>
+      <c r="AJ2" s="29"/>
+      <c r="AK2" s="29"/>
+      <c r="AL2" s="29"/>
+      <c r="AM2" s="29"/>
+      <c r="AN2" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="AO2" s="22"/>
-      <c r="AP2" s="22"/>
-      <c r="AQ2" s="22"/>
-      <c r="AR2" s="22"/>
-      <c r="AS2" s="22"/>
-      <c r="AT2" s="22"/>
-      <c r="AU2" s="22"/>
-      <c r="AV2" s="22"/>
-      <c r="AW2" s="22"/>
-      <c r="AX2" s="22"/>
-      <c r="AY2" s="22"/>
-      <c r="AZ2" s="22"/>
-      <c r="BA2" s="22"/>
-      <c r="BB2" s="22"/>
-      <c r="BC2" s="22"/>
-      <c r="BD2" s="22"/>
-      <c r="BE2" s="22"/>
-      <c r="BF2" s="22"/>
-      <c r="BG2" s="22"/>
-      <c r="BH2" s="22"/>
-      <c r="BI2" s="22"/>
-      <c r="BJ2" s="22"/>
-      <c r="BK2" s="22"/>
-      <c r="BL2" s="26"/>
-      <c r="BM2" s="26"/>
-      <c r="BN2" s="26"/>
-      <c r="BO2" s="26"/>
-      <c r="BP2" s="26"/>
-      <c r="BQ2" s="26"/>
-      <c r="BR2" s="26"/>
-      <c r="BS2" s="26"/>
-      <c r="BT2" s="26"/>
-      <c r="BU2" s="26"/>
-      <c r="BV2" s="26"/>
-      <c r="BW2" s="26"/>
-      <c r="BX2" s="26"/>
-      <c r="BY2" s="26"/>
-      <c r="BZ2" s="26"/>
-      <c r="CA2" s="26"/>
-      <c r="CB2" s="26"/>
-      <c r="CC2" s="26"/>
-      <c r="CD2" s="26"/>
-      <c r="CE2" s="26"/>
-      <c r="CF2" s="26"/>
-      <c r="CG2" s="26"/>
-      <c r="CH2" s="26"/>
-      <c r="CI2" s="26"/>
+      <c r="AO2" s="29"/>
+      <c r="AP2" s="29"/>
+      <c r="AQ2" s="29"/>
+      <c r="AR2" s="29"/>
+      <c r="AS2" s="29"/>
+      <c r="AT2" s="29"/>
+      <c r="AU2" s="29"/>
+      <c r="AV2" s="29"/>
+      <c r="AW2" s="29"/>
+      <c r="AX2" s="29"/>
+      <c r="AY2" s="29"/>
+      <c r="AZ2" s="29"/>
+      <c r="BA2" s="29"/>
+      <c r="BB2" s="29"/>
+      <c r="BC2" s="29"/>
+      <c r="BD2" s="29"/>
+      <c r="BE2" s="29"/>
+      <c r="BF2" s="29"/>
+      <c r="BG2" s="29"/>
+      <c r="BH2" s="29"/>
+      <c r="BI2" s="29"/>
+      <c r="BJ2" s="29"/>
+      <c r="BK2" s="29"/>
+      <c r="BL2" s="36"/>
+      <c r="BM2" s="36"/>
+      <c r="BN2" s="36"/>
+      <c r="BO2" s="36"/>
+      <c r="BP2" s="36"/>
+      <c r="BQ2" s="36"/>
+      <c r="BR2" s="36"/>
+      <c r="BS2" s="36"/>
+      <c r="BT2" s="36"/>
+      <c r="BU2" s="36"/>
+      <c r="BV2" s="36"/>
+      <c r="BW2" s="36"/>
+      <c r="BX2" s="36"/>
+      <c r="BY2" s="36"/>
+      <c r="BZ2" s="36"/>
+      <c r="CA2" s="36"/>
+      <c r="CB2" s="36"/>
+      <c r="CC2" s="36"/>
+      <c r="CD2" s="36"/>
+      <c r="CE2" s="36"/>
+      <c r="CF2" s="36"/>
+      <c r="CG2" s="36"/>
+      <c r="CH2" s="36"/>
+      <c r="CI2" s="36"/>
     </row>
-    <row r="3" ht="15" customHeight="1" spans="1:87">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="13" t="s">
+    <row r="3" spans="1:87" ht="15" customHeight="1">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="K3" s="13"/>
-      <c r="L3" s="13"/>
-      <c r="M3" s="13"/>
-      <c r="N3" s="13"/>
-      <c r="O3" s="13"/>
-      <c r="P3" s="13" t="s">
+      <c r="K3" s="37"/>
+      <c r="L3" s="37"/>
+      <c r="M3" s="37"/>
+      <c r="N3" s="37"/>
+      <c r="O3" s="37"/>
+      <c r="P3" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="Q3" s="13"/>
-      <c r="R3" s="13"/>
-      <c r="S3" s="13"/>
-      <c r="T3" s="13"/>
-      <c r="U3" s="13"/>
-      <c r="V3" s="13" t="s">
+      <c r="Q3" s="37"/>
+      <c r="R3" s="37"/>
+      <c r="S3" s="37"/>
+      <c r="T3" s="37"/>
+      <c r="U3" s="37"/>
+      <c r="V3" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="W3" s="13"/>
-      <c r="X3" s="13"/>
-      <c r="Y3" s="13"/>
-      <c r="Z3" s="13"/>
-      <c r="AA3" s="13"/>
-      <c r="AB3" s="13" t="s">
+      <c r="W3" s="37"/>
+      <c r="X3" s="37"/>
+      <c r="Y3" s="37"/>
+      <c r="Z3" s="37"/>
+      <c r="AA3" s="37"/>
+      <c r="AB3" s="37" t="s">
         <v>18</v>
       </c>
-      <c r="AC3" s="13"/>
-      <c r="AD3" s="13"/>
-      <c r="AE3" s="13"/>
-      <c r="AF3" s="13"/>
-      <c r="AG3" s="13"/>
-      <c r="AH3" s="13" t="s">
+      <c r="AC3" s="37"/>
+      <c r="AD3" s="37"/>
+      <c r="AE3" s="37"/>
+      <c r="AF3" s="37"/>
+      <c r="AG3" s="37"/>
+      <c r="AH3" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="AI3" s="13"/>
-      <c r="AJ3" s="13"/>
-      <c r="AK3" s="13"/>
-      <c r="AL3" s="13"/>
-      <c r="AM3" s="13"/>
-      <c r="AN3" s="13" t="s">
+      <c r="AI3" s="37"/>
+      <c r="AJ3" s="37"/>
+      <c r="AK3" s="37"/>
+      <c r="AL3" s="37"/>
+      <c r="AM3" s="37"/>
+      <c r="AN3" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="AO3" s="13"/>
-      <c r="AP3" s="13"/>
-      <c r="AQ3" s="13"/>
-      <c r="AR3" s="13"/>
-      <c r="AS3" s="13"/>
-      <c r="AT3" s="13" t="s">
+      <c r="AO3" s="37"/>
+      <c r="AP3" s="37"/>
+      <c r="AQ3" s="37"/>
+      <c r="AR3" s="37"/>
+      <c r="AS3" s="37"/>
+      <c r="AT3" s="37" t="s">
         <v>21</v>
       </c>
-      <c r="AU3" s="13"/>
-      <c r="AV3" s="13"/>
-      <c r="AW3" s="13"/>
-      <c r="AX3" s="13"/>
-      <c r="AY3" s="13"/>
-      <c r="AZ3" s="13" t="s">
+      <c r="AU3" s="37"/>
+      <c r="AV3" s="37"/>
+      <c r="AW3" s="37"/>
+      <c r="AX3" s="37"/>
+      <c r="AY3" s="37"/>
+      <c r="AZ3" s="37" t="s">
         <v>22</v>
       </c>
-      <c r="BA3" s="13"/>
-      <c r="BB3" s="13"/>
-      <c r="BC3" s="13"/>
-      <c r="BD3" s="13"/>
-      <c r="BE3" s="13"/>
-      <c r="BF3" s="13" t="s">
+      <c r="BA3" s="37"/>
+      <c r="BB3" s="37"/>
+      <c r="BC3" s="37"/>
+      <c r="BD3" s="37"/>
+      <c r="BE3" s="37"/>
+      <c r="BF3" s="37" t="s">
         <v>23</v>
       </c>
-      <c r="BG3" s="13"/>
-      <c r="BH3" s="13"/>
-      <c r="BI3" s="13"/>
-      <c r="BJ3" s="13"/>
-      <c r="BK3" s="13"/>
-      <c r="BL3" s="13" t="s">
+      <c r="BG3" s="37"/>
+      <c r="BH3" s="37"/>
+      <c r="BI3" s="37"/>
+      <c r="BJ3" s="37"/>
+      <c r="BK3" s="37"/>
+      <c r="BL3" s="37" t="s">
         <v>24</v>
       </c>
-      <c r="BM3" s="13"/>
-      <c r="BN3" s="13"/>
-      <c r="BO3" s="13"/>
-      <c r="BP3" s="13"/>
-      <c r="BQ3" s="13"/>
-      <c r="BR3" s="13" t="s">
+      <c r="BM3" s="37"/>
+      <c r="BN3" s="37"/>
+      <c r="BO3" s="37"/>
+      <c r="BP3" s="37"/>
+      <c r="BQ3" s="37"/>
+      <c r="BR3" s="37" t="s">
         <v>25</v>
       </c>
-      <c r="BS3" s="13"/>
-      <c r="BT3" s="13"/>
-      <c r="BU3" s="13"/>
-      <c r="BV3" s="13"/>
-      <c r="BW3" s="13"/>
-      <c r="BX3" s="13" t="s">
+      <c r="BS3" s="37"/>
+      <c r="BT3" s="37"/>
+      <c r="BU3" s="37"/>
+      <c r="BV3" s="37"/>
+      <c r="BW3" s="37"/>
+      <c r="BX3" s="37" t="s">
         <v>26</v>
       </c>
-      <c r="BY3" s="13"/>
-      <c r="BZ3" s="13"/>
-      <c r="CA3" s="13"/>
-      <c r="CB3" s="13"/>
-      <c r="CC3" s="13"/>
-      <c r="CD3" s="13" t="s">
+      <c r="BY3" s="37"/>
+      <c r="BZ3" s="37"/>
+      <c r="CA3" s="37"/>
+      <c r="CB3" s="37"/>
+      <c r="CC3" s="37"/>
+      <c r="CD3" s="37" t="s">
         <v>27</v>
       </c>
-      <c r="CE3" s="13"/>
-      <c r="CF3" s="13"/>
-      <c r="CG3" s="13"/>
-      <c r="CH3" s="13"/>
-      <c r="CI3" s="13"/>
+      <c r="CE3" s="37"/>
+      <c r="CF3" s="37"/>
+      <c r="CG3" s="37"/>
+      <c r="CH3" s="37"/>
+      <c r="CI3" s="37"/>
     </row>
-    <row r="4" spans="1:87">
-      <c r="A4" s="4" t="s">
+    <row r="4" spans="1:87" ht="15.75">
+      <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="F4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="G4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="H4" s="4" t="s">
+      <c r="H4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="I4" s="4" t="s">
+      <c r="I4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="J4" s="23" t="s">
+      <c r="J4" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="K4" s="23" t="s">
+      <c r="K4" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="L4" s="23" t="s">
+      <c r="L4" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="M4" s="23" t="s">
+      <c r="M4" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="N4" s="23" t="s">
+      <c r="N4" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="O4" s="23" t="s">
+      <c r="O4" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="P4" s="23" t="s">
+      <c r="P4" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="Q4" s="23" t="s">
+      <c r="Q4" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="R4" s="23" t="s">
+      <c r="R4" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="S4" s="23" t="s">
+      <c r="S4" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="T4" s="23" t="s">
+      <c r="T4" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="U4" s="23" t="s">
+      <c r="U4" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="V4" s="23" t="s">
+      <c r="V4" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="W4" s="23" t="s">
+      <c r="W4" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="X4" s="23" t="s">
+      <c r="X4" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="Y4" s="23" t="s">
+      <c r="Y4" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="Z4" s="23" t="s">
+      <c r="Z4" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="AA4" s="23" t="s">
+      <c r="AA4" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="AB4" s="23" t="s">
+      <c r="AB4" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="AC4" s="23" t="s">
+      <c r="AC4" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="AD4" s="23" t="s">
+      <c r="AD4" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="AE4" s="23" t="s">
+      <c r="AE4" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="AF4" s="23" t="s">
+      <c r="AF4" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="AG4" s="23" t="s">
+      <c r="AG4" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="AH4" s="23" t="s">
+      <c r="AH4" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="AI4" s="23" t="s">
+      <c r="AI4" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="AJ4" s="23" t="s">
+      <c r="AJ4" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="AK4" s="23" t="s">
+      <c r="AK4" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="AL4" s="23" t="s">
+      <c r="AL4" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="AM4" s="23" t="s">
+      <c r="AM4" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="AN4" s="23" t="s">
+      <c r="AN4" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="AO4" s="23" t="s">
+      <c r="AO4" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="AP4" s="23" t="s">
+      <c r="AP4" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="AQ4" s="23" t="s">
+      <c r="AQ4" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="AR4" s="23" t="s">
+      <c r="AR4" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="AS4" s="23" t="s">
+      <c r="AS4" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="AT4" s="23" t="s">
+      <c r="AT4" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="AU4" s="23" t="s">
+      <c r="AU4" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="AV4" s="23" t="s">
+      <c r="AV4" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="AW4" s="23" t="s">
+      <c r="AW4" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="AX4" s="23" t="s">
+      <c r="AX4" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="AY4" s="23" t="s">
+      <c r="AY4" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="AZ4" s="23" t="s">
+      <c r="AZ4" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="BA4" s="23" t="s">
+      <c r="BA4" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="BB4" s="23" t="s">
+      <c r="BB4" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="BC4" s="23" t="s">
+      <c r="BC4" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="BD4" s="23" t="s">
+      <c r="BD4" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="BE4" s="23" t="s">
+      <c r="BE4" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="BF4" s="23" t="s">
+      <c r="BF4" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="BG4" s="23" t="s">
+      <c r="BG4" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="BH4" s="23" t="s">
+      <c r="BH4" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="BI4" s="23" t="s">
+      <c r="BI4" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="BJ4" s="23" t="s">
+      <c r="BJ4" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="BK4" s="23" t="s">
+      <c r="BK4" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="BL4" s="23" t="s">
+      <c r="BL4" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="BM4" s="23" t="s">
+      <c r="BM4" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="BN4" s="23" t="s">
+      <c r="BN4" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="BO4" s="23" t="s">
+      <c r="BO4" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="BP4" s="23" t="s">
+      <c r="BP4" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="BQ4" s="23" t="s">
+      <c r="BQ4" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="BR4" s="23" t="s">
+      <c r="BR4" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="BS4" s="23" t="s">
+      <c r="BS4" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="BT4" s="23" t="s">
+      <c r="BT4" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="BU4" s="23" t="s">
+      <c r="BU4" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="BV4" s="23" t="s">
+      <c r="BV4" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="BW4" s="23" t="s">
+      <c r="BW4" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="BX4" s="23" t="s">
+      <c r="BX4" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="BY4" s="23" t="s">
+      <c r="BY4" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="BZ4" s="23" t="s">
+      <c r="BZ4" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="CA4" s="23" t="s">
+      <c r="CA4" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="CB4" s="23" t="s">
+      <c r="CB4" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="CC4" s="23" t="s">
+      <c r="CC4" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="CD4" s="23" t="s">
+      <c r="CD4" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="CE4" s="23" t="s">
+      <c r="CE4" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="CF4" s="23" t="s">
+      <c r="CF4" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="CG4" s="23" t="s">
+      <c r="CG4" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="CH4" s="23" t="s">
+      <c r="CH4" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="CI4" s="23" t="s">
+      <c r="CI4" s="16" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:87">
-      <c r="A5" s="18">
+      <c r="A5" s="12">
         <v>11000465</v>
       </c>
-      <c r="B5" s="19" t="s">
+      <c r="B5" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="C5" s="19" t="s">
+      <c r="C5" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="D5" s="19" t="s">
+      <c r="D5" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="E5" s="19" t="s">
+      <c r="E5" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="F5" s="19" t="s">
+      <c r="F5" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="G5" s="19" t="s">
+      <c r="G5" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="H5" s="19" t="s">
+      <c r="H5" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="I5" s="24" t="s">
+      <c r="I5" s="17" t="s">
         <v>35</v>
       </c>
       <c r="J5">
@@ -2811,31 +2192,31 @@
       </c>
     </row>
     <row r="6" spans="1:87">
-      <c r="A6" s="20">
+      <c r="A6" s="14">
         <v>11000201</v>
       </c>
-      <c r="B6" s="21" t="s">
+      <c r="B6" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="C6" s="21" t="s">
+      <c r="C6" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="D6" s="21" t="s">
+      <c r="D6" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="E6" s="21" t="s">
+      <c r="E6" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="F6" s="21" t="s">
+      <c r="F6" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="G6" s="21" t="s">
+      <c r="G6" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="H6" s="21" t="s">
+      <c r="H6" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="I6" s="25" t="s">
+      <c r="I6" s="18" t="s">
         <v>38</v>
       </c>
       <c r="J6">
@@ -3074,31 +2455,31 @@
       </c>
     </row>
     <row r="7" spans="1:87">
-      <c r="A7" s="20">
+      <c r="A7" s="14">
         <v>11000260</v>
       </c>
-      <c r="B7" s="21" t="s">
+      <c r="B7" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="21" t="s">
+      <c r="C7" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="D7" s="21" t="s">
+      <c r="D7" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="E7" s="21" t="s">
+      <c r="E7" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="F7" s="21" t="s">
+      <c r="F7" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="G7" s="21" t="s">
+      <c r="G7" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="H7" s="21" t="s">
+      <c r="H7" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="I7" s="25" t="s">
+      <c r="I7" s="18" t="s">
         <v>38</v>
       </c>
       <c r="J7">
@@ -3337,31 +2718,31 @@
       </c>
     </row>
     <row r="8" spans="1:87">
-      <c r="A8" s="20">
+      <c r="A8" s="14">
         <v>11000317</v>
       </c>
-      <c r="B8" s="21" t="s">
+      <c r="B8" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="21" t="s">
+      <c r="C8" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="D8" s="21" t="s">
+      <c r="D8" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="E8" s="21" t="s">
+      <c r="E8" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="F8" s="21" t="s">
+      <c r="F8" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="G8" s="21" t="s">
+      <c r="G8" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="H8" s="21" t="s">
+      <c r="H8" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="I8" s="25" t="s">
+      <c r="I8" s="18" t="s">
         <v>38</v>
       </c>
       <c r="J8">
@@ -3601,6 +2982,19 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="BR3:BW3"/>
+    <mergeCell ref="BX3:CC3"/>
+    <mergeCell ref="CD3:CI3"/>
+    <mergeCell ref="AN3:AS3"/>
+    <mergeCell ref="AT3:AY3"/>
+    <mergeCell ref="AZ3:BE3"/>
+    <mergeCell ref="BF3:BK3"/>
+    <mergeCell ref="BL3:BQ3"/>
+    <mergeCell ref="J3:O3"/>
+    <mergeCell ref="P3:U3"/>
+    <mergeCell ref="V3:AA3"/>
+    <mergeCell ref="AB3:AG3"/>
+    <mergeCell ref="AH3:AM3"/>
     <mergeCell ref="A1:I1"/>
     <mergeCell ref="J1:BK1"/>
     <mergeCell ref="BL1:CI1"/>
@@ -3608,46 +3002,31 @@
     <mergeCell ref="J2:AM2"/>
     <mergeCell ref="AN2:BK2"/>
     <mergeCell ref="BL2:CI2"/>
-    <mergeCell ref="J3:O3"/>
-    <mergeCell ref="P3:U3"/>
-    <mergeCell ref="V3:AA3"/>
-    <mergeCell ref="AB3:AG3"/>
-    <mergeCell ref="AH3:AM3"/>
-    <mergeCell ref="AN3:AS3"/>
-    <mergeCell ref="AT3:AY3"/>
-    <mergeCell ref="AZ3:BE3"/>
-    <mergeCell ref="BF3:BK3"/>
-    <mergeCell ref="BL3:BQ3"/>
-    <mergeCell ref="BR3:BW3"/>
-    <mergeCell ref="BX3:CC3"/>
-    <mergeCell ref="CD3:CI3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="portrait"/>
-  <headerFooter/>
+  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AI8"/>
   <sheetViews>
     <sheetView topLeftCell="F1" workbookViewId="0">
       <selection activeCell="I4" sqref="A4:I4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83333333333333" defaultRowHeight="15.75" outlineLevelRow="7"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="19.6666666666667" customWidth="1"/>
-    <col min="2" max="2" width="11.1666666666667" customWidth="1"/>
-    <col min="3" max="3" width="10.8333333333333" customWidth="1"/>
-    <col min="4" max="4" width="15.8333333333333" customWidth="1"/>
-    <col min="5" max="5" width="11.5" customWidth="1"/>
-    <col min="6" max="6" width="42.3333333333333" customWidth="1"/>
-    <col min="7" max="7" width="13.6666666666667" customWidth="1"/>
-    <col min="8" max="8" width="17.5" customWidth="1"/>
-    <col min="9" max="9" width="21.1666666666667" customWidth="1"/>
+    <col min="1" max="1" width="19.7109375" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" customWidth="1"/>
+    <col min="4" max="4" width="15.85546875" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" customWidth="1"/>
+    <col min="6" max="6" width="42.28515625" customWidth="1"/>
+    <col min="7" max="7" width="13.7109375" customWidth="1"/>
+    <col min="8" max="8" width="17.42578125" customWidth="1"/>
+    <col min="9" max="9" width="21.140625" customWidth="1"/>
     <col min="10" max="10" width="11" customWidth="1"/>
     <col min="11" max="11" width="10" customWidth="1"/>
     <col min="12" max="12" width="11" customWidth="1"/>
@@ -3674,447 +3053,447 @@
     <col min="33" max="33" width="10" customWidth="1"/>
     <col min="34" max="34" width="11" customWidth="1"/>
     <col min="35" max="35" width="10" customWidth="1"/>
-    <col min="36" max="36" width="5.83333333333333" customWidth="1"/>
-    <col min="37" max="37" width="6.33333333333333" customWidth="1"/>
-    <col min="38" max="38" width="8.66666666666667" customWidth="1"/>
+    <col min="36" max="36" width="5.85546875" customWidth="1"/>
+    <col min="37" max="37" width="6.28515625" customWidth="1"/>
+    <col min="38" max="38" width="8.7109375" customWidth="1"/>
     <col min="39" max="39" width="9" customWidth="1"/>
-    <col min="40" max="40" width="14.5" customWidth="1"/>
-    <col min="41" max="41" width="7.5" customWidth="1"/>
-    <col min="42" max="42" width="5.83333333333333" customWidth="1"/>
-    <col min="43" max="43" width="6.33333333333333" customWidth="1"/>
-    <col min="44" max="44" width="8.66666666666667" customWidth="1"/>
+    <col min="40" max="40" width="14.42578125" customWidth="1"/>
+    <col min="41" max="41" width="7.42578125" customWidth="1"/>
+    <col min="42" max="42" width="5.85546875" customWidth="1"/>
+    <col min="43" max="43" width="6.28515625" customWidth="1"/>
+    <col min="44" max="44" width="8.7109375" customWidth="1"/>
     <col min="45" max="45" width="9" customWidth="1"/>
-    <col min="46" max="46" width="14.5" customWidth="1"/>
-    <col min="47" max="47" width="7.5" customWidth="1"/>
-    <col min="48" max="48" width="5.83333333333333" customWidth="1"/>
-    <col min="49" max="49" width="6.33333333333333" customWidth="1"/>
-    <col min="50" max="50" width="8.66666666666667" customWidth="1"/>
+    <col min="46" max="46" width="14.42578125" customWidth="1"/>
+    <col min="47" max="47" width="7.42578125" customWidth="1"/>
+    <col min="48" max="48" width="5.85546875" customWidth="1"/>
+    <col min="49" max="49" width="6.28515625" customWidth="1"/>
+    <col min="50" max="50" width="8.7109375" customWidth="1"/>
     <col min="51" max="51" width="9" customWidth="1"/>
-    <col min="52" max="52" width="14.5" customWidth="1"/>
-    <col min="53" max="53" width="7.5" customWidth="1"/>
-    <col min="54" max="54" width="5.83333333333333" customWidth="1"/>
-    <col min="55" max="55" width="6.33333333333333" customWidth="1"/>
-    <col min="56" max="56" width="8.66666666666667" customWidth="1"/>
+    <col min="52" max="52" width="14.42578125" customWidth="1"/>
+    <col min="53" max="53" width="7.42578125" customWidth="1"/>
+    <col min="54" max="54" width="5.85546875" customWidth="1"/>
+    <col min="55" max="55" width="6.28515625" customWidth="1"/>
+    <col min="56" max="56" width="8.7109375" customWidth="1"/>
     <col min="57" max="57" width="9" customWidth="1"/>
-    <col min="58" max="58" width="14.5" customWidth="1"/>
-    <col min="59" max="59" width="7.5" customWidth="1"/>
-    <col min="60" max="60" width="5.83333333333333" customWidth="1"/>
-    <col min="61" max="61" width="6.33333333333333" customWidth="1"/>
-    <col min="62" max="62" width="8.66666666666667" customWidth="1"/>
+    <col min="58" max="58" width="14.42578125" customWidth="1"/>
+    <col min="59" max="59" width="7.42578125" customWidth="1"/>
+    <col min="60" max="60" width="5.85546875" customWidth="1"/>
+    <col min="61" max="61" width="6.28515625" customWidth="1"/>
+    <col min="62" max="62" width="8.7109375" customWidth="1"/>
     <col min="63" max="63" width="9" customWidth="1"/>
-    <col min="64" max="64" width="14.5" customWidth="1"/>
-    <col min="65" max="65" width="7.5" customWidth="1"/>
-    <col min="66" max="66" width="5.83333333333333" customWidth="1"/>
-    <col min="67" max="67" width="6.33333333333333" customWidth="1"/>
-    <col min="68" max="68" width="8.66666666666667" customWidth="1"/>
+    <col min="64" max="64" width="14.42578125" customWidth="1"/>
+    <col min="65" max="65" width="7.42578125" customWidth="1"/>
+    <col min="66" max="66" width="5.85546875" customWidth="1"/>
+    <col min="67" max="67" width="6.28515625" customWidth="1"/>
+    <col min="68" max="68" width="8.7109375" customWidth="1"/>
     <col min="69" max="69" width="9" customWidth="1"/>
-    <col min="70" max="70" width="14.5" customWidth="1"/>
-    <col min="71" max="71" width="7.5" customWidth="1"/>
-    <col min="72" max="72" width="5.83333333333333" customWidth="1"/>
-    <col min="73" max="73" width="6.33333333333333" customWidth="1"/>
-    <col min="74" max="74" width="8.66666666666667" customWidth="1"/>
+    <col min="70" max="70" width="14.42578125" customWidth="1"/>
+    <col min="71" max="71" width="7.42578125" customWidth="1"/>
+    <col min="72" max="72" width="5.85546875" customWidth="1"/>
+    <col min="73" max="73" width="6.28515625" customWidth="1"/>
+    <col min="74" max="74" width="8.7109375" customWidth="1"/>
     <col min="75" max="75" width="9" customWidth="1"/>
-    <col min="76" max="76" width="14.5" customWidth="1"/>
-    <col min="77" max="77" width="7.5" customWidth="1"/>
-    <col min="78" max="78" width="5.83333333333333" customWidth="1"/>
-    <col min="79" max="79" width="6.33333333333333" customWidth="1"/>
-    <col min="80" max="80" width="8.66666666666667" customWidth="1"/>
+    <col min="76" max="76" width="14.42578125" customWidth="1"/>
+    <col min="77" max="77" width="7.42578125" customWidth="1"/>
+    <col min="78" max="78" width="5.85546875" customWidth="1"/>
+    <col min="79" max="79" width="6.28515625" customWidth="1"/>
+    <col min="80" max="80" width="8.7109375" customWidth="1"/>
     <col min="81" max="81" width="9" customWidth="1"/>
-    <col min="82" max="82" width="14.5" customWidth="1"/>
-    <col min="83" max="83" width="7.5" customWidth="1"/>
-    <col min="84" max="84" width="5.83333333333333" customWidth="1"/>
-    <col min="85" max="85" width="6.33333333333333" customWidth="1"/>
-    <col min="86" max="86" width="8.66666666666667" customWidth="1"/>
+    <col min="82" max="82" width="14.42578125" customWidth="1"/>
+    <col min="83" max="83" width="7.42578125" customWidth="1"/>
+    <col min="84" max="84" width="5.85546875" customWidth="1"/>
+    <col min="85" max="85" width="6.28515625" customWidth="1"/>
+    <col min="86" max="86" width="8.7109375" customWidth="1"/>
     <col min="87" max="87" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15" customHeight="1" spans="1:35">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:35" ht="15" customHeight="1">
+      <c r="A1" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="9" t="s">
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
+      <c r="I1" s="34"/>
+      <c r="J1" s="38" t="s">
         <v>49</v>
       </c>
-      <c r="K1" s="9"/>
-      <c r="L1" s="9"/>
-      <c r="M1" s="9"/>
-      <c r="N1" s="9"/>
-      <c r="O1" s="9"/>
-      <c r="P1" s="9"/>
-      <c r="Q1" s="9"/>
-      <c r="R1" s="9"/>
-      <c r="S1" s="9"/>
-      <c r="T1" s="9"/>
-      <c r="U1" s="9"/>
-      <c r="V1" s="9"/>
-      <c r="W1" s="9"/>
-      <c r="X1" s="9"/>
-      <c r="Y1" s="9"/>
-      <c r="Z1" s="9"/>
-      <c r="AA1" s="9"/>
-      <c r="AB1" s="13" t="s">
+      <c r="K1" s="38"/>
+      <c r="L1" s="38"/>
+      <c r="M1" s="38"/>
+      <c r="N1" s="38"/>
+      <c r="O1" s="38"/>
+      <c r="P1" s="38"/>
+      <c r="Q1" s="38"/>
+      <c r="R1" s="38"/>
+      <c r="S1" s="38"/>
+      <c r="T1" s="38"/>
+      <c r="U1" s="38"/>
+      <c r="V1" s="38"/>
+      <c r="W1" s="38"/>
+      <c r="X1" s="38"/>
+      <c r="Y1" s="38"/>
+      <c r="Z1" s="38"/>
+      <c r="AA1" s="38"/>
+      <c r="AB1" s="37" t="s">
         <v>42</v>
       </c>
-      <c r="AC1" s="13"/>
-      <c r="AD1" s="13"/>
-      <c r="AE1" s="13"/>
-      <c r="AF1" s="13"/>
-      <c r="AG1" s="13"/>
-      <c r="AH1" s="13"/>
-      <c r="AI1" s="13"/>
+      <c r="AC1" s="37"/>
+      <c r="AD1" s="37"/>
+      <c r="AE1" s="37"/>
+      <c r="AF1" s="37"/>
+      <c r="AG1" s="37"/>
+      <c r="AH1" s="37"/>
+      <c r="AI1" s="37"/>
     </row>
-    <row r="2" ht="15" customHeight="1" spans="1:35">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="9" t="s">
+    <row r="2" spans="1:35" ht="15" customHeight="1">
+      <c r="A2" s="35"/>
+      <c r="B2" s="35"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="35"/>
+      <c r="I2" s="35"/>
+      <c r="J2" s="38" t="s">
         <v>50</v>
       </c>
-      <c r="K2" s="9"/>
-      <c r="L2" s="9"/>
-      <c r="M2" s="9"/>
-      <c r="N2" s="9"/>
-      <c r="O2" s="9"/>
-      <c r="P2" s="9"/>
-      <c r="Q2" s="9"/>
-      <c r="R2" s="9"/>
-      <c r="S2" s="9"/>
-      <c r="T2" s="9" t="s">
+      <c r="K2" s="38"/>
+      <c r="L2" s="38"/>
+      <c r="M2" s="38"/>
+      <c r="N2" s="38"/>
+      <c r="O2" s="38"/>
+      <c r="P2" s="38"/>
+      <c r="Q2" s="38"/>
+      <c r="R2" s="38"/>
+      <c r="S2" s="38"/>
+      <c r="T2" s="38" t="s">
         <v>51</v>
       </c>
-      <c r="U2" s="9"/>
-      <c r="V2" s="9"/>
-      <c r="W2" s="9"/>
-      <c r="X2" s="9"/>
-      <c r="Y2" s="9"/>
-      <c r="Z2" s="9"/>
-      <c r="AA2" s="9"/>
-      <c r="AB2" s="14"/>
-      <c r="AC2" s="16"/>
-      <c r="AD2" s="16"/>
-      <c r="AE2" s="16"/>
-      <c r="AF2" s="16"/>
-      <c r="AG2" s="16"/>
-      <c r="AH2" s="16"/>
-      <c r="AI2" s="17"/>
+      <c r="U2" s="38"/>
+      <c r="V2" s="38"/>
+      <c r="W2" s="38"/>
+      <c r="X2" s="38"/>
+      <c r="Y2" s="38"/>
+      <c r="Z2" s="38"/>
+      <c r="AA2" s="38"/>
+      <c r="AB2" s="39"/>
+      <c r="AC2" s="40"/>
+      <c r="AD2" s="40"/>
+      <c r="AE2" s="40"/>
+      <c r="AF2" s="40"/>
+      <c r="AG2" s="40"/>
+      <c r="AH2" s="40"/>
+      <c r="AI2" s="41"/>
     </row>
-    <row r="3" ht="15" customHeight="1" spans="1:35">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="9" t="s">
+    <row r="3" spans="1:35" ht="15" customHeight="1">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="38" t="s">
         <v>52</v>
       </c>
-      <c r="K3" s="9"/>
-      <c r="L3" s="9" t="s">
+      <c r="K3" s="38"/>
+      <c r="L3" s="38" t="s">
         <v>16</v>
       </c>
-      <c r="M3" s="9"/>
-      <c r="N3" s="9" t="s">
+      <c r="M3" s="38"/>
+      <c r="N3" s="38" t="s">
         <v>17</v>
       </c>
-      <c r="O3" s="9"/>
-      <c r="P3" s="9" t="s">
+      <c r="O3" s="38"/>
+      <c r="P3" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="Q3" s="9"/>
-      <c r="R3" s="9" t="s">
+      <c r="Q3" s="38"/>
+      <c r="R3" s="38" t="s">
         <v>19</v>
       </c>
-      <c r="S3" s="9"/>
-      <c r="T3" s="9" t="s">
+      <c r="S3" s="38"/>
+      <c r="T3" s="38" t="s">
         <v>20</v>
       </c>
-      <c r="U3" s="9"/>
-      <c r="V3" s="9" t="s">
+      <c r="U3" s="38"/>
+      <c r="V3" s="38" t="s">
         <v>21</v>
       </c>
-      <c r="W3" s="9"/>
-      <c r="X3" s="9" t="s">
+      <c r="W3" s="38"/>
+      <c r="X3" s="38" t="s">
         <v>22</v>
       </c>
-      <c r="Y3" s="9"/>
-      <c r="Z3" s="9" t="s">
+      <c r="Y3" s="38"/>
+      <c r="Z3" s="38" t="s">
         <v>23</v>
       </c>
-      <c r="AA3" s="9"/>
-      <c r="AB3" s="13" t="s">
+      <c r="AA3" s="38"/>
+      <c r="AB3" s="37" t="s">
         <v>24</v>
       </c>
-      <c r="AC3" s="13"/>
-      <c r="AD3" s="13" t="s">
+      <c r="AC3" s="37"/>
+      <c r="AD3" s="37" t="s">
         <v>25</v>
       </c>
-      <c r="AE3" s="13"/>
-      <c r="AF3" s="13" t="s">
+      <c r="AE3" s="37"/>
+      <c r="AF3" s="37" t="s">
         <v>26</v>
       </c>
-      <c r="AG3" s="13"/>
-      <c r="AH3" s="13" t="s">
+      <c r="AG3" s="37"/>
+      <c r="AH3" s="37" t="s">
         <v>27</v>
       </c>
-      <c r="AI3" s="13"/>
+      <c r="AI3" s="37"/>
     </row>
-    <row r="4" spans="1:35">
-      <c r="A4" s="4" t="s">
+    <row r="4" spans="1:35" ht="15.75">
+      <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="F4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="G4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="H4" s="4" t="s">
+      <c r="H4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="I4" s="4" t="s">
+      <c r="I4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="J4" s="10" t="s">
+      <c r="J4" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="K4" s="10" t="s">
+      <c r="K4" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="L4" s="10" t="s">
+      <c r="L4" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="M4" s="10" t="s">
+      <c r="M4" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="N4" s="10" t="s">
+      <c r="N4" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="O4" s="10" t="s">
+      <c r="O4" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="P4" s="10" t="s">
+      <c r="P4" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="Q4" s="10" t="s">
+      <c r="Q4" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="R4" s="10" t="s">
+      <c r="R4" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="S4" s="10" t="s">
+      <c r="S4" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="T4" s="10" t="s">
+      <c r="T4" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="U4" s="10" t="s">
+      <c r="U4" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="V4" s="10" t="s">
+      <c r="V4" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="W4" s="10" t="s">
+      <c r="W4" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="X4" s="10" t="s">
+      <c r="X4" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="Y4" s="10" t="s">
+      <c r="Y4" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="Z4" s="10" t="s">
+      <c r="Z4" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="AA4" s="10" t="s">
+      <c r="AA4" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="AB4" s="15" t="s">
+      <c r="AB4" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="AC4" s="15" t="s">
+      <c r="AC4" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="AD4" s="15" t="s">
+      <c r="AD4" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="AE4" s="15" t="s">
+      <c r="AE4" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="AF4" s="15" t="s">
+      <c r="AF4" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="AG4" s="15" t="s">
+      <c r="AG4" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="AH4" s="15" t="s">
+      <c r="AH4" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="AI4" s="15" t="s">
+      <c r="AI4" s="11" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:35">
-      <c r="A5" s="5">
+      <c r="A5" s="3">
         <v>11000465</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="F5" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="G5" s="6" t="s">
+      <c r="G5" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="H5" s="6" t="s">
+      <c r="H5" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="I5" s="6" t="s">
+      <c r="I5" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="J5" s="11">
-        <v>1</v>
-      </c>
-      <c r="K5" s="11">
-        <v>1</v>
-      </c>
-      <c r="L5" s="11">
-        <v>1</v>
-      </c>
-      <c r="M5" s="11">
-        <v>1</v>
-      </c>
-      <c r="N5" s="11">
-        <v>1</v>
-      </c>
-      <c r="O5" s="11">
-        <v>1</v>
-      </c>
-      <c r="P5" s="11">
-        <v>1</v>
-      </c>
-      <c r="Q5" s="11">
-        <v>1</v>
-      </c>
-      <c r="R5" s="11">
-        <v>1</v>
-      </c>
-      <c r="S5" s="11">
-        <v>1</v>
-      </c>
-      <c r="T5" s="11">
-        <v>1</v>
-      </c>
-      <c r="U5" s="11">
-        <v>1</v>
-      </c>
-      <c r="V5" s="11">
-        <v>1</v>
-      </c>
-      <c r="W5" s="11">
-        <v>1</v>
-      </c>
-      <c r="X5" s="11">
-        <v>1</v>
-      </c>
-      <c r="Y5" s="11">
-        <v>1</v>
-      </c>
-      <c r="Z5" s="11">
-        <v>1</v>
-      </c>
-      <c r="AA5" s="11">
-        <v>1</v>
-      </c>
-      <c r="AB5" s="11">
-        <v>1</v>
-      </c>
-      <c r="AC5" s="11">
-        <v>1</v>
-      </c>
-      <c r="AD5" s="11">
-        <v>1</v>
-      </c>
-      <c r="AE5" s="11">
-        <v>1</v>
-      </c>
-      <c r="AF5" s="11">
-        <v>1</v>
-      </c>
-      <c r="AG5" s="11">
-        <v>1</v>
-      </c>
-      <c r="AH5" s="11">
-        <v>1</v>
-      </c>
-      <c r="AI5" s="11">
+      <c r="J5" s="8">
+        <v>1</v>
+      </c>
+      <c r="K5" s="8">
+        <v>1</v>
+      </c>
+      <c r="L5" s="8">
+        <v>1</v>
+      </c>
+      <c r="M5" s="8">
+        <v>1</v>
+      </c>
+      <c r="N5" s="8">
+        <v>1</v>
+      </c>
+      <c r="O5" s="8">
+        <v>1</v>
+      </c>
+      <c r="P5" s="8">
+        <v>1</v>
+      </c>
+      <c r="Q5" s="8">
+        <v>1</v>
+      </c>
+      <c r="R5" s="8">
+        <v>1</v>
+      </c>
+      <c r="S5" s="8">
+        <v>1</v>
+      </c>
+      <c r="T5" s="8">
+        <v>1</v>
+      </c>
+      <c r="U5" s="8">
+        <v>1</v>
+      </c>
+      <c r="V5" s="8">
+        <v>1</v>
+      </c>
+      <c r="W5" s="8">
+        <v>1</v>
+      </c>
+      <c r="X5" s="8">
+        <v>1</v>
+      </c>
+      <c r="Y5" s="8">
+        <v>1</v>
+      </c>
+      <c r="Z5" s="8">
+        <v>1</v>
+      </c>
+      <c r="AA5" s="8">
+        <v>1</v>
+      </c>
+      <c r="AB5" s="8">
+        <v>1</v>
+      </c>
+      <c r="AC5" s="8">
+        <v>1</v>
+      </c>
+      <c r="AD5" s="8">
+        <v>1</v>
+      </c>
+      <c r="AE5" s="8">
+        <v>1</v>
+      </c>
+      <c r="AF5" s="8">
+        <v>1</v>
+      </c>
+      <c r="AG5" s="8">
+        <v>1</v>
+      </c>
+      <c r="AH5" s="8">
+        <v>1</v>
+      </c>
+      <c r="AI5" s="8">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:35">
-      <c r="A6" s="7">
+      <c r="A6" s="5">
         <v>11000201</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="D6" s="8">
+      <c r="D6" s="6">
         <v>1100205</v>
       </c>
-      <c r="E6" s="8" t="s">
+      <c r="E6" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="F6" s="8" t="s">
+      <c r="F6" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="G6" s="8" t="s">
+      <c r="G6" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="H6" s="8" t="s">
+      <c r="H6" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="I6" s="12" t="s">
+      <c r="I6" s="9" t="s">
         <v>38</v>
       </c>
       <c r="J6">
@@ -4197,106 +3576,106 @@
       </c>
     </row>
     <row r="7" spans="1:35">
-      <c r="A7" s="7">
+      <c r="A7" s="5">
         <v>11000260</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="D7" s="8">
+      <c r="D7" s="6">
         <v>1100205</v>
       </c>
-      <c r="E7" s="8" t="s">
+      <c r="E7" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="F7" s="8" t="s">
+      <c r="F7" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="G7" s="8" t="s">
+      <c r="G7" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="H7" s="8" t="s">
+      <c r="H7" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="I7" s="12" t="s">
+      <c r="I7" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="J7" s="11">
+      <c r="J7" s="8">
         <v>3</v>
       </c>
       <c r="K7">
         <v>4</v>
       </c>
-      <c r="L7" s="11">
+      <c r="L7" s="8">
         <v>5</v>
       </c>
       <c r="M7">
         <v>6</v>
       </c>
-      <c r="N7" s="11">
+      <c r="N7" s="8">
         <v>7</v>
       </c>
       <c r="O7">
         <v>8</v>
       </c>
-      <c r="P7" s="11">
+      <c r="P7" s="8">
         <v>9</v>
       </c>
       <c r="Q7">
         <v>10</v>
       </c>
-      <c r="R7" s="11">
+      <c r="R7" s="8">
         <v>11</v>
       </c>
       <c r="S7">
         <v>12</v>
       </c>
-      <c r="T7" s="11">
+      <c r="T7" s="8">
         <v>13</v>
       </c>
       <c r="U7">
         <v>14</v>
       </c>
-      <c r="V7" s="11">
+      <c r="V7" s="8">
         <v>15</v>
       </c>
       <c r="W7">
         <v>16</v>
       </c>
-      <c r="X7" s="11">
+      <c r="X7" s="8">
         <v>17</v>
       </c>
       <c r="Y7">
         <v>18</v>
       </c>
-      <c r="Z7" s="11">
+      <c r="Z7" s="8">
         <v>19</v>
       </c>
       <c r="AA7">
         <v>20</v>
       </c>
-      <c r="AB7" s="11">
+      <c r="AB7" s="8">
         <v>21</v>
       </c>
       <c r="AC7">
         <v>22</v>
       </c>
-      <c r="AD7" s="11">
+      <c r="AD7" s="8">
         <v>23</v>
       </c>
       <c r="AE7">
         <v>24</v>
       </c>
-      <c r="AF7" s="11">
+      <c r="AF7" s="8">
         <v>25</v>
       </c>
       <c r="AG7">
         <v>26</v>
       </c>
-      <c r="AH7" s="11">
+      <c r="AH7" s="8">
         <v>27</v>
       </c>
       <c r="AI7">
@@ -4304,31 +3683,31 @@
       </c>
     </row>
     <row r="8" spans="1:35">
-      <c r="A8" s="7">
+      <c r="A8" s="5">
         <v>11000317</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="D8" s="8">
+      <c r="D8" s="6">
         <v>1100205</v>
       </c>
-      <c r="E8" s="8" t="s">
+      <c r="E8" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="F8" s="8" t="s">
+      <c r="F8" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="G8" s="8" t="s">
+      <c r="G8" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="H8" s="8" t="s">
+      <c r="H8" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="I8" s="12" t="s">
+      <c r="I8" s="9" t="s">
         <v>38</v>
       </c>
       <c r="J8">
@@ -4412,6 +3791,19 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="AD3:AE3"/>
+    <mergeCell ref="AF3:AG3"/>
+    <mergeCell ref="AH3:AI3"/>
+    <mergeCell ref="T3:U3"/>
+    <mergeCell ref="V3:W3"/>
+    <mergeCell ref="X3:Y3"/>
+    <mergeCell ref="Z3:AA3"/>
+    <mergeCell ref="AB3:AC3"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="L3:M3"/>
+    <mergeCell ref="N3:O3"/>
+    <mergeCell ref="P3:Q3"/>
+    <mergeCell ref="R3:S3"/>
     <mergeCell ref="A1:I1"/>
     <mergeCell ref="J1:AA1"/>
     <mergeCell ref="AB1:AI1"/>
@@ -4419,21 +3811,7 @@
     <mergeCell ref="J2:S2"/>
     <mergeCell ref="T2:AA2"/>
     <mergeCell ref="AB2:AI2"/>
-    <mergeCell ref="J3:K3"/>
-    <mergeCell ref="L3:M3"/>
-    <mergeCell ref="N3:O3"/>
-    <mergeCell ref="P3:Q3"/>
-    <mergeCell ref="R3:S3"/>
-    <mergeCell ref="T3:U3"/>
-    <mergeCell ref="V3:W3"/>
-    <mergeCell ref="X3:Y3"/>
-    <mergeCell ref="Z3:AA3"/>
-    <mergeCell ref="AB3:AC3"/>
-    <mergeCell ref="AD3:AE3"/>
-    <mergeCell ref="AF3:AG3"/>
-    <mergeCell ref="AH3:AI3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Acrescimo de novos campos no arquivo XLS de teste
</commit_message>
<xml_diff>
--- a/Modelos_V2/tabela1_padrao_matricula.xlsx
+++ b/Modelos_V2/tabela1_padrao_matricula.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mansouza\Documents\www\TrajetoriaEscolar\Modelos_V2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{CF7200C0-B6E2-4745-9B62-5435C8296E80}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{A3EAB2BE-3C2E-4CBD-80ED-26BB16A1E5C5}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12945" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12945" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Matrículas-Total" sheetId="1" r:id="rId1"/>
@@ -813,7 +813,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
@@ -1267,8 +1267,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:CI8"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>

</xml_diff>